<commit_message>
Did lots of work on the Jupyter Notebooks. Tried my best to move xlwings to pandas. Still need to do some work on the reference Jupyter Notebook.
</commit_message>
<xml_diff>
--- a/Old_Materials/L8--Python xlwings/sudoku_puzzle.xlsx
+++ b/Old_Materials/L8--Python xlwings/sudoku_puzzle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skipper/Dropbox/usna/courses_usna/SA405/SA405_fall_ay21/Lessons_AY21/L8--Python xlwings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcurry/Desktop/SA405/Old_Materials/L8--Python xlwings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B4E260-999F-534F-9367-E2828853AE17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEFBD6C-350C-EC4E-9FF3-4E9F73128E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{688CD8B8-7CB8-AC49-B678-F43DC54A0870}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="20540" activeTab="1" xr2:uid="{688CD8B8-7CB8-AC49-B678-F43DC54A0870}"/>
   </bookViews>
   <sheets>
     <sheet name="Solution1" sheetId="15" r:id="rId1"/>
@@ -821,10 +821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C472F138-57D0-A14A-8F1D-FAA95C3D9C57}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I10" sqref="A2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,22 +832,7 @@
     <col min="1" max="19" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3">
-        <v>9</v>
-      </c>
+    <row r="1" spans="1:20" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
@@ -859,20 +844,22 @@
       <c r="S1" s="10"/>
       <c r="T1" s="11"/>
     </row>
-    <row r="2" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6"/>
+    <row r="2" spans="1:20" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3">
+        <v>9</v>
+      </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -884,22 +871,20 @@
       <c r="S2" s="10"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:20" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8">
-        <v>8</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8">
-        <v>7</v>
-      </c>
-      <c r="I3" s="9"/>
+    <row r="3" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
@@ -911,24 +896,22 @@
       <c r="S3" s="10"/>
       <c r="T3" s="11"/>
     </row>
-    <row r="4" spans="1:20" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3">
+    <row r="4" spans="1:20" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8">
         <v>7</v>
       </c>
-      <c r="G4" s="1">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="9"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -940,22 +923,24 @@
       <c r="S4" s="10"/>
       <c r="T4" s="11"/>
     </row>
-    <row r="5" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4">
-        <v>4</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
+    <row r="5" spans="1:20" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -967,24 +952,22 @@
       <c r="S5" s="10"/>
       <c r="T5" s="11"/>
     </row>
-    <row r="6" spans="1:20" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>8</v>
-      </c>
-      <c r="D6" s="7">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8">
-        <v>4</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
+    <row r="6" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="4">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -996,22 +979,24 @@
       <c r="S6" s="10"/>
       <c r="T6" s="11"/>
     </row>
-    <row r="7" spans="1:20" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="1">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
+    <row r="7" spans="1:20" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -1023,20 +1008,22 @@
       <c r="S7" s="10"/>
       <c r="T7" s="11"/>
     </row>
-    <row r="8" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5">
-        <v>9</v>
-      </c>
-      <c r="I8" s="6"/>
+    <row r="8" spans="1:20" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1048,20 +1035,20 @@
       <c r="S8" s="10"/>
       <c r="T8" s="11"/>
     </row>
-    <row r="9" spans="1:20" ht="32" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7">
-        <v>6</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
+    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5">
+        <v>9</v>
+      </c>
+      <c r="I9" s="6"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -1073,7 +1060,22 @@
       <c r="S9" s="10"/>
       <c r="T9" s="11"/>
     </row>
-    <row r="10" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:20" ht="32" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="7">
+        <v>6</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>